<commit_message>
update 2FA authentication script
</commit_message>
<xml_diff>
--- a/SFM-SDM-WebAutomation/src/main/java/resources/externalData/credsData.xlsx
+++ b/SFM-SDM-WebAutomation/src/main/java/resources/externalData/credsData.xlsx
@@ -156,13 +156,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.36"/>
@@ -202,9 +202,9 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>